<commit_message>
Renew own vocab list.
</commit_message>
<xml_diff>
--- a/Vocab_grabbed_on_the_way.xlsx
+++ b/Vocab_grabbed_on_the_way.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yxk\Documents\github\gre_resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF945BEF-6E98-46B7-B416-03959B6D54E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0066FB39-39DF-4622-AEDA-818D95101F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21850" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="668">
   <si>
     <t>word</t>
   </si>
@@ -1985,6 +1985,96 @@
   </si>
   <si>
     <t>n. 无误；教皇永无谬误论</t>
+  </si>
+  <si>
+    <t>immunity</t>
+  </si>
+  <si>
+    <t>n. 免疫力；豁免权；免除</t>
+  </si>
+  <si>
+    <t>impartially</t>
+  </si>
+  <si>
+    <t>adv. 公平地；无私地</t>
+  </si>
+  <si>
+    <t>remedial</t>
+  </si>
+  <si>
+    <t>adj. 治疗的；补救的；矫正的</t>
+  </si>
+  <si>
+    <t>discomfit</t>
+  </si>
+  <si>
+    <t>vt. 挫败；扰乱，破坏；使…为难；使…破灭</t>
+  </si>
+  <si>
+    <t>expedient</t>
+  </si>
+  <si>
+    <t>adj. 权宜的；方便的；有利的</t>
+  </si>
+  <si>
+    <t>n. 权宜之计；应急手段</t>
+  </si>
+  <si>
+    <t>reside</t>
+  </si>
+  <si>
+    <t>vi. 住，居住；属于</t>
+  </si>
+  <si>
+    <t>comet</t>
+  </si>
+  <si>
+    <t>n. [天] 彗星</t>
+  </si>
+  <si>
+    <t>elliptical</t>
+  </si>
+  <si>
+    <t>adj. 椭圆的；省略的</t>
+  </si>
+  <si>
+    <t>slingshot</t>
+  </si>
+  <si>
+    <t>n. 弹弓</t>
+  </si>
+  <si>
+    <t>munificence</t>
+  </si>
+  <si>
+    <t>n. 慷慨给与；宽宏大量</t>
+  </si>
+  <si>
+    <t>inure</t>
+  </si>
+  <si>
+    <t>bode</t>
+  </si>
+  <si>
+    <t>vt. 预示；为…的兆头</t>
+  </si>
+  <si>
+    <t>sting</t>
+  </si>
+  <si>
+    <t>vt. 刺；驱使；使…苦恼；使…疼痛</t>
+  </si>
+  <si>
+    <t>vt. 使…习惯；使…适应</t>
+  </si>
+  <si>
+    <t>deviously</t>
+  </si>
+  <si>
+    <t>adv. 绕道地；弯曲地</t>
+  </si>
+  <si>
+    <t>craftily</t>
   </si>
 </sst>
 </file>
@@ -2321,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD340"/>
+  <dimension ref="A1:XFD356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B340" sqref="B340"/>
+    <sheetView tabSelected="1" topLeftCell="A324" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4975,6 +5065,131 @@
       </c>
       <c r="B340" t="s">
         <v>637</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>638</v>
+      </c>
+      <c r="B341" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>640</v>
+      </c>
+      <c r="B342" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>642</v>
+      </c>
+      <c r="B343" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>644</v>
+      </c>
+      <c r="B344" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>646</v>
+      </c>
+      <c r="B345" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B346" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>649</v>
+      </c>
+      <c r="B347" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>651</v>
+      </c>
+      <c r="B348" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
+        <v>653</v>
+      </c>
+      <c r="B349" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
+        <v>655</v>
+      </c>
+      <c r="B350" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
+        <v>657</v>
+      </c>
+      <c r="B351" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
+        <v>659</v>
+      </c>
+      <c r="B352" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
+        <v>660</v>
+      </c>
+      <c r="B353" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
+        <v>662</v>
+      </c>
+      <c r="B354" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
+        <v>665</v>
+      </c>
+      <c r="B355" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>667</v>
+      </c>
+      <c r="B356" t="s">
+        <v>667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>